<commit_message>
All Test Class Include
</commit_message>
<xml_diff>
--- a/ATS_HR/ExcelFiles/ATS_Login_1.xlsx
+++ b/ATS_HR/ExcelFiles/ATS_Login_1.xlsx
@@ -13,30 +13,132 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="42">
   <si>
     <t>UN</t>
   </si>
   <si>
-    <t>PW</t>
-  </si>
-  <si>
-    <t>Kunal</t>
-  </si>
-  <si>
-    <t>Vivek</t>
-  </si>
-  <si>
-    <t>Hitesh</t>
+    <t>PWD</t>
+  </si>
+  <si>
+    <t>hitesh</t>
+  </si>
+  <si>
+    <t>hitesh@123</t>
+  </si>
+  <si>
+    <t>manish</t>
+  </si>
+  <si>
+    <t>manish@123</t>
+  </si>
+  <si>
+    <t>ketan</t>
+  </si>
+  <si>
+    <t>ketan@123</t>
   </si>
   <si>
     <t>ashingote</t>
   </si>
   <si>
+    <t>pass</t>
+  </si>
+  <si>
     <t>fail</t>
   </si>
   <si>
-    <t>pass</t>
+    <t>pass--1575382299967</t>
+  </si>
+  <si>
+    <t>fail--1575382311547</t>
+  </si>
+  <si>
+    <t>pass--1575382325924</t>
+  </si>
+  <si>
+    <t>pass--1575382338392</t>
+  </si>
+  <si>
+    <t>pass--1575382588327</t>
+  </si>
+  <si>
+    <t>pass--1575382588443</t>
+  </si>
+  <si>
+    <t>pass--1575382588491</t>
+  </si>
+  <si>
+    <t>pass--1575382588526</t>
+  </si>
+  <si>
+    <t>fail--1575382600020</t>
+  </si>
+  <si>
+    <t>fail--1575382600082</t>
+  </si>
+  <si>
+    <t>fail--1575382600114</t>
+  </si>
+  <si>
+    <t>fail--1575382600144</t>
+  </si>
+  <si>
+    <t>pass--1575382612777</t>
+  </si>
+  <si>
+    <t>pass--1575382612808</t>
+  </si>
+  <si>
+    <t>pass--1575382612854</t>
+  </si>
+  <si>
+    <t>pass--1575382612895</t>
+  </si>
+  <si>
+    <t>pass--1575382625537</t>
+  </si>
+  <si>
+    <t>pass--1575382625572</t>
+  </si>
+  <si>
+    <t>pass--1575382625620</t>
+  </si>
+  <si>
+    <t>pass--1575382625659</t>
+  </si>
+  <si>
+    <t>pass--1575387425562</t>
+  </si>
+  <si>
+    <t>fail--1575387437235</t>
+  </si>
+  <si>
+    <t>pass--1575387449615</t>
+  </si>
+  <si>
+    <t>pass--1575387462410</t>
+  </si>
+  <si>
+    <t>pass--1575387528211</t>
+  </si>
+  <si>
+    <t>fail--1575387539862</t>
+  </si>
+  <si>
+    <t>pass--1575387552433</t>
+  </si>
+  <si>
+    <t>pass--1575387564844</t>
+  </si>
+  <si>
+    <t>pass--1575387802591</t>
+  </si>
+  <si>
+    <t>pass--1575387852661</t>
+  </si>
+  <si>
+    <t>pass--1575387953070</t>
   </si>
 </sst>
 </file>
@@ -44,26 +146,34 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font/>
+    <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <color rgb="FF000000"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -72,15 +182,18 @@
   <cellStyleXfs count="1">
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+      <alignment readingOrder="0"/>
     </xf>
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -293,18 +406,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="9.71" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="10.57" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="18.14" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="9.29" collapsed="true"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -318,53 +424,45 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
+      <c r="A3" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>